<commit_message>
chnaged backend structure for personal,diagnosis
</commit_message>
<xml_diff>
--- a/notes.xlsx
+++ b/notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Work\Blockchain_projects\Medchain\Rough\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC137F9E-5964-4512-B5CD-857B0454C7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90390585-EF55-4890-95EA-9689F697DC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{A2A8DC1D-16AC-499C-9A7F-A38B80E348A6}"/>
+    <workbookView xWindow="6930" yWindow="3675" windowWidth="28800" windowHeight="15555" activeTab="2" xr2:uid="{A2A8DC1D-16AC-499C-9A7F-A38B80E348A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract Creation" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Create Contract All Steps</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>getContractobject</t>
+  </si>
+  <si>
+    <t>/approvals/:id</t>
+  </si>
+  <si>
+    <t>agreementController.approveAgreement</t>
+  </si>
+  <si>
+    <t>approveAgreement function</t>
+  </si>
+  <si>
+    <t>approveAgreement</t>
   </si>
 </sst>
 </file>
@@ -796,8 +808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F355671C-032F-410F-9A46-96E4797DE9AA}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,12 +907,102 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D076AA-2D88-46BF-B75B-C54304993572}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="47.85546875" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" customWidth="1"/>
+    <col min="7" max="7" width="35.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="6"/>
+      <c r="H10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>